<commit_message>
Login Page Test script with data provider
</commit_message>
<xml_diff>
--- a/resources/testdata/Demo.xlsx
+++ b/resources/testdata/Demo.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>password</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>ms103@gmail.com</t>
+  </si>
+  <si>
+    <t>UserEmail</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>automation101@gmail.com</t>
+  </si>
+  <si>
+    <t>automation101</t>
   </si>
 </sst>
 </file>
@@ -425,7 +437,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -565,14 +577,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>